<commit_message>
real datas access out
</commit_message>
<xml_diff>
--- a/Projetos/Projetos 2015/relatorioCasos/_suplementos/base-dados-2015/setembro/relatoriosCasos-set.xlsx
+++ b/Projetos/Projetos 2015/relatorioCasos/_suplementos/base-dados-2015/setembro/relatoriosCasos-set.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="0" windowWidth="30140" windowHeight="21100" tabRatio="500"/>
+    <workbookView xWindow="14960" yWindow="480" windowWidth="30140" windowHeight="21100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="set" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -8965,7 +8965,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:B38" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -9481,15 +9481,15 @@
   <dimension ref="A1:F634"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F634"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.5" customWidth="1"/>
+    <col min="4" max="4" width="63.5" customWidth="1"/>
     <col min="5" max="5" width="52.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
@@ -9514,7 +9514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="1" t="s">
         <v>1217</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>42248.392638888887</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="1" t="s">
         <v>1207</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>42248.437395833331</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="1" t="s">
         <v>1207</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>42248.5078125</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="1" t="s">
         <v>1198</v>
       </c>
@@ -9854,7 +9854,7 @@
         <v>42248.681319444448</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="1" t="s">
         <v>563</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>42248.763761574075</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="30">
       <c r="A24" s="1" t="s">
         <v>1168</v>
       </c>
@@ -10094,7 +10094,7 @@
         <v>42248.894988425927</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="30">
       <c r="A31" s="1" t="s">
         <v>1156</v>
       </c>
@@ -10114,7 +10114,7 @@
         <v>42248.89671296296</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="1" t="s">
         <v>1153</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>42249.61173611111</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" ht="30">
       <c r="A47" s="1" t="s">
         <v>1128</v>
       </c>
@@ -10814,7 +10814,7 @@
         <v>42250.587766203702</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" ht="30">
       <c r="A67" s="1" t="s">
         <v>1089</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>42250.724062499998</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" ht="30">
       <c r="A77" s="1" t="s">
         <v>1066</v>
       </c>
@@ -11234,7 +11234,7 @@
         <v>42251.520543981482</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" ht="30">
       <c r="A88" s="1" t="s">
         <v>1046</v>
       </c>
@@ -11514,7 +11514,7 @@
         <v>42251.921458333331</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" ht="30">
       <c r="A102" s="1" t="s">
         <v>1010</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>42254.366828703707</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" ht="30">
       <c r="A115" s="1" t="s">
         <v>984</v>
       </c>
@@ -12694,7 +12694,7 @@
         <v>42256.725983796299</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" ht="30">
       <c r="A161" s="1" t="s">
         <v>897</v>
       </c>
@@ -12814,7 +12814,7 @@
         <v>42256.738449074073</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" ht="30">
       <c r="A167" s="1" t="s">
         <v>897</v>
       </c>
@@ -13074,7 +13074,7 @@
         <v>42257.397858796299</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" ht="30">
       <c r="A180" s="1" t="s">
         <v>882</v>
       </c>
@@ -13094,7 +13094,7 @@
         <v>42257.398333333331</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" ht="30">
       <c r="A181" s="1" t="s">
         <v>882</v>
       </c>
@@ -13134,7 +13134,7 @@
         <v>42257.429386574076</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" ht="30">
       <c r="A183" s="1" t="s">
         <v>882</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>42257.43681712963</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" ht="30">
       <c r="A187" s="1" t="s">
         <v>882</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>42257.87027777778</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" ht="30">
       <c r="A204" s="1" t="s">
         <v>848</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>42257.916574074072</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" ht="30">
       <c r="A207" s="1" t="s">
         <v>844</v>
       </c>
@@ -13694,7 +13694,7 @@
         <v>42257.932291666664</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" ht="30">
       <c r="A211" s="1" t="s">
         <v>838</v>
       </c>
@@ -13994,7 +13994,7 @@
         <v>42258.850046296298</v>
       </c>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:6" ht="30">
       <c r="A226" s="1" t="s">
         <v>805</v>
       </c>
@@ -14034,7 +14034,7 @@
         <v>42259.409930555557</v>
       </c>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:6" ht="30">
       <c r="A228" s="1" t="s">
         <v>799</v>
       </c>
@@ -14154,7 +14154,7 @@
         <v>42260.386886574073</v>
       </c>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:6" ht="30">
       <c r="A234" s="1" t="s">
         <v>789</v>
       </c>
@@ -14294,7 +14294,7 @@
         <v>42260.856064814812</v>
       </c>
     </row>
-    <row r="241" spans="1:6">
+    <row r="241" spans="1:6" ht="30">
       <c r="A241" s="1" t="s">
         <v>769</v>
       </c>
@@ -14334,7 +14334,7 @@
         <v>42260.874131944445</v>
       </c>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:6" ht="30">
       <c r="A243" s="1" t="s">
         <v>772</v>
       </c>
@@ -14354,7 +14354,7 @@
         <v>42260.879178240742</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:6" ht="30">
       <c r="A244" s="1" t="s">
         <v>769</v>
       </c>
@@ -14434,7 +14434,7 @@
         <v>42261.035520833335</v>
       </c>
     </row>
-    <row r="248" spans="1:6">
+    <row r="248" spans="1:6" ht="30">
       <c r="A248" s="1" t="s">
         <v>757</v>
       </c>
@@ -14514,7 +14514,7 @@
         <v>42261.038784722223</v>
       </c>
     </row>
-    <row r="252" spans="1:6">
+    <row r="252" spans="1:6" ht="30">
       <c r="A252" s="1" t="s">
         <v>757</v>
       </c>
@@ -14534,7 +14534,7 @@
         <v>42261.03943287037</v>
       </c>
     </row>
-    <row r="253" spans="1:6">
+    <row r="253" spans="1:6" ht="30">
       <c r="A253" s="1" t="s">
         <v>757</v>
       </c>
@@ -14674,7 +14674,7 @@
         <v>42261.503159722219</v>
       </c>
     </row>
-    <row r="260" spans="1:6">
+    <row r="260" spans="1:6" ht="30">
       <c r="A260" s="1" t="s">
         <v>745</v>
       </c>
@@ -14914,7 +14914,7 @@
         <v>42261.909803240742</v>
       </c>
     </row>
-    <row r="272" spans="1:6">
+    <row r="272" spans="1:6" ht="30">
       <c r="A272" s="1" t="s">
         <v>716</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>42261.91097222222</v>
       </c>
     </row>
-    <row r="273" spans="1:6">
+    <row r="273" spans="1:6" ht="30">
       <c r="A273" s="1" t="s">
         <v>716</v>
       </c>
@@ -15094,7 +15094,7 @@
         <v>42261.917222222219</v>
       </c>
     </row>
-    <row r="281" spans="1:6">
+    <row r="281" spans="1:6" ht="30">
       <c r="A281" s="1" t="s">
         <v>716</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>42261.917928240742</v>
       </c>
     </row>
-    <row r="282" spans="1:6">
+    <row r="282" spans="1:6" ht="30">
       <c r="A282" s="1" t="s">
         <v>716</v>
       </c>
@@ -15234,7 +15234,7 @@
         <v>42261.922777777778</v>
       </c>
     </row>
-    <row r="288" spans="1:6">
+    <row r="288" spans="1:6" ht="30">
       <c r="A288" s="1" t="s">
         <v>716</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>42261.927766203706</v>
       </c>
     </row>
-    <row r="293" spans="1:6">
+    <row r="293" spans="1:6" ht="30">
       <c r="A293" s="1" t="s">
         <v>716</v>
       </c>
@@ -15374,7 +15374,7 @@
         <v>42261.929942129631</v>
       </c>
     </row>
-    <row r="295" spans="1:6">
+    <row r="295" spans="1:6" ht="30">
       <c r="A295" s="1" t="s">
         <v>716</v>
       </c>
@@ -15474,7 +15474,7 @@
         <v>42262.443078703705</v>
       </c>
     </row>
-    <row r="300" spans="1:6">
+    <row r="300" spans="1:6" ht="30">
       <c r="A300" s="1" t="s">
         <v>682</v>
       </c>
@@ -15534,7 +15534,7 @@
         <v>42262.532175925924</v>
       </c>
     </row>
-    <row r="303" spans="1:6">
+    <row r="303" spans="1:6" ht="30">
       <c r="A303" s="1" t="s">
         <v>699</v>
       </c>
@@ -15914,7 +15914,7 @@
         <v>42263.350451388891</v>
       </c>
     </row>
-    <row r="322" spans="1:6">
+    <row r="322" spans="1:6" ht="30">
       <c r="A322" s="1" t="s">
         <v>656</v>
       </c>
@@ -16074,7 +16074,7 @@
         <v>42263.633449074077</v>
       </c>
     </row>
-    <row r="330" spans="1:6">
+    <row r="330" spans="1:6" ht="30">
       <c r="A330" s="1" t="s">
         <v>636</v>
       </c>
@@ -16434,7 +16434,7 @@
         <v>42264.732314814813</v>
       </c>
     </row>
-    <row r="348" spans="1:6">
+    <row r="348" spans="1:6" ht="30">
       <c r="A348" s="1" t="s">
         <v>594</v>
       </c>
@@ -16594,7 +16594,7 @@
         <v>42264.815046296295</v>
       </c>
     </row>
-    <row r="356" spans="1:6">
+    <row r="356" spans="1:6" ht="30">
       <c r="A356" s="1" t="s">
         <v>580</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>42264.853298611109</v>
       </c>
     </row>
-    <row r="359" spans="1:6">
+    <row r="359" spans="1:6" ht="30">
       <c r="A359" s="1" t="s">
         <v>574</v>
       </c>
@@ -16714,7 +16714,7 @@
         <v>42265.294039351851</v>
       </c>
     </row>
-    <row r="362" spans="1:6">
+    <row r="362" spans="1:6" ht="30">
       <c r="A362" s="1" t="s">
         <v>572</v>
       </c>
@@ -16874,7 +16874,7 @@
         <v>42265.568414351852</v>
       </c>
     </row>
-    <row r="370" spans="1:6">
+    <row r="370" spans="1:6" ht="30">
       <c r="A370" s="1" t="s">
         <v>563</v>
       </c>
@@ -17074,7 +17074,7 @@
         <v>42265.729861111111</v>
       </c>
     </row>
-    <row r="380" spans="1:6">
+    <row r="380" spans="1:6" ht="30">
       <c r="A380" s="1" t="s">
         <v>552</v>
       </c>
@@ -17174,7 +17174,7 @@
         <v>42265.958321759259</v>
       </c>
     </row>
-    <row r="385" spans="1:6">
+    <row r="385" spans="1:6" ht="30">
       <c r="A385" s="1" t="s">
         <v>540</v>
       </c>
@@ -17194,7 +17194,7 @@
         <v>42265.960277777776</v>
       </c>
     </row>
-    <row r="386" spans="1:6">
+    <row r="386" spans="1:6" ht="30">
       <c r="A386" s="1" t="s">
         <v>540</v>
       </c>
@@ -17234,7 +17234,7 @@
         <v>42265.962812500002</v>
       </c>
     </row>
-    <row r="388" spans="1:6">
+    <row r="388" spans="1:6" ht="30">
       <c r="A388" s="1" t="s">
         <v>534</v>
       </c>
@@ -17334,7 +17334,7 @@
         <v>42267.485601851855</v>
       </c>
     </row>
-    <row r="393" spans="1:6">
+    <row r="393" spans="1:6" ht="30">
       <c r="A393" s="1" t="s">
         <v>521</v>
       </c>
@@ -17594,7 +17594,7 @@
         <v>42268.410833333335</v>
       </c>
     </row>
-    <row r="406" spans="1:6">
+    <row r="406" spans="1:6" ht="30">
       <c r="A406" s="1" t="s">
         <v>488</v>
       </c>
@@ -17794,7 +17794,7 @@
         <v>42268.465057870373</v>
       </c>
     </row>
-    <row r="416" spans="1:6">
+    <row r="416" spans="1:6" ht="30">
       <c r="A416" s="1" t="s">
         <v>482</v>
       </c>
@@ -17934,7 +17934,7 @@
         <v>42268.619409722225</v>
       </c>
     </row>
-    <row r="423" spans="1:6">
+    <row r="423" spans="1:6" ht="30">
       <c r="A423" s="1" t="s">
         <v>471</v>
       </c>
@@ -17954,7 +17954,7 @@
         <v>42268.619895833333</v>
       </c>
     </row>
-    <row r="424" spans="1:6">
+    <row r="424" spans="1:6" ht="30">
       <c r="A424" s="1" t="s">
         <v>468</v>
       </c>
@@ -18334,7 +18334,7 @@
         <v>42268.984166666669</v>
       </c>
     </row>
-    <row r="443" spans="1:6">
+    <row r="443" spans="1:6" ht="30">
       <c r="A443" s="1" t="s">
         <v>427</v>
       </c>
@@ -18674,7 +18674,7 @@
         <v>42269.723541666666</v>
       </c>
     </row>
-    <row r="460" spans="1:6">
+    <row r="460" spans="1:6" ht="30">
       <c r="A460" s="1" t="s">
         <v>400</v>
       </c>
@@ -19094,7 +19094,7 @@
         <v>42270.600972222222</v>
       </c>
     </row>
-    <row r="481" spans="1:6">
+    <row r="481" spans="1:6" ht="30">
       <c r="A481" s="1" t="s">
         <v>367</v>
       </c>
@@ -19154,7 +19154,7 @@
         <v>42270.645289351851</v>
       </c>
     </row>
-    <row r="484" spans="1:6">
+    <row r="484" spans="1:6" ht="30">
       <c r="A484" s="1" t="s">
         <v>184</v>
       </c>
@@ -19274,7 +19274,7 @@
         <v>42270.711365740739</v>
       </c>
     </row>
-    <row r="490" spans="1:6">
+    <row r="490" spans="1:6" ht="30">
       <c r="A490" s="1" t="s">
         <v>354</v>
       </c>
@@ -19314,7 +19314,7 @@
         <v>42270.999571759261</v>
       </c>
     </row>
-    <row r="492" spans="1:6">
+    <row r="492" spans="1:6" ht="30">
       <c r="A492" s="1" t="s">
         <v>349</v>
       </c>
@@ -19434,7 +19434,7 @@
         <v>42271.581967592596</v>
       </c>
     </row>
-    <row r="498" spans="1:6">
+    <row r="498" spans="1:6" ht="30">
       <c r="A498" s="1" t="s">
         <v>331</v>
       </c>
@@ -19614,7 +19614,7 @@
         <v>42271.743159722224</v>
       </c>
     </row>
-    <row r="507" spans="1:6">
+    <row r="507" spans="1:6" ht="30">
       <c r="A507" s="1" t="s">
         <v>313</v>
       </c>
@@ -19694,7 +19694,7 @@
         <v>42271.847268518519</v>
       </c>
     </row>
-    <row r="511" spans="1:6">
+    <row r="511" spans="1:6" ht="30">
       <c r="A511" s="1" t="s">
         <v>252</v>
       </c>
@@ -19774,7 +19774,7 @@
         <v>42271.86042824074</v>
       </c>
     </row>
-    <row r="515" spans="1:6">
+    <row r="515" spans="1:6" ht="30">
       <c r="A515" s="1" t="s">
         <v>298</v>
       </c>
@@ -19934,7 +19934,7 @@
         <v>42272.428599537037</v>
       </c>
     </row>
-    <row r="523" spans="1:6">
+    <row r="523" spans="1:6" ht="30">
       <c r="A523" s="1" t="s">
         <v>278</v>
       </c>
@@ -19954,7 +19954,7 @@
         <v>42272.431875000002</v>
       </c>
     </row>
-    <row r="524" spans="1:6">
+    <row r="524" spans="1:6" ht="30">
       <c r="A524" s="1" t="s">
         <v>282</v>
       </c>
@@ -20074,7 +20074,7 @@
         <v>42272.689699074072</v>
       </c>
     </row>
-    <row r="530" spans="1:6">
+    <row r="530" spans="1:6" ht="30">
       <c r="A530" s="1" t="s">
         <v>268</v>
       </c>
@@ -20194,7 +20194,7 @@
         <v>42273.570729166669</v>
       </c>
     </row>
-    <row r="536" spans="1:6">
+    <row r="536" spans="1:6" ht="30">
       <c r="A536" s="1" t="s">
         <v>252</v>
       </c>
@@ -20454,7 +20454,7 @@
         <v>42274.523032407407</v>
       </c>
     </row>
-    <row r="549" spans="1:6">
+    <row r="549" spans="1:6" ht="30">
       <c r="A549" s="1" t="s">
         <v>225</v>
       </c>
@@ -20914,7 +20914,7 @@
         <v>42275.642789351848</v>
       </c>
     </row>
-    <row r="572" spans="1:6">
+    <row r="572" spans="1:6" ht="30">
       <c r="A572" s="1" t="s">
         <v>184</v>
       </c>
@@ -20934,7 +20934,7 @@
         <v>42275.645486111112</v>
       </c>
     </row>
-    <row r="573" spans="1:6">
+    <row r="573" spans="1:6" ht="30">
       <c r="A573" s="1" t="s">
         <v>181</v>
       </c>
@@ -20974,7 +20974,7 @@
         <v>42275.675428240742</v>
       </c>
     </row>
-    <row r="575" spans="1:6">
+    <row r="575" spans="1:6" ht="30">
       <c r="A575" s="1" t="s">
         <v>177</v>
       </c>
@@ -21234,7 +21234,7 @@
         <v>42276.435173611113</v>
       </c>
     </row>
-    <row r="588" spans="1:6">
+    <row r="588" spans="1:6" ht="30">
       <c r="A588" s="1" t="s">
         <v>140</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v>42276.469328703701</v>
       </c>
     </row>
-    <row r="592" spans="1:6">
+    <row r="592" spans="1:6" ht="30">
       <c r="A592" s="1" t="s">
         <v>128</v>
       </c>
@@ -21454,7 +21454,7 @@
         <v>42276.60125</v>
       </c>
     </row>
-    <row r="599" spans="1:6">
+    <row r="599" spans="1:6" ht="30">
       <c r="A599" s="1" t="s">
         <v>114</v>
       </c>
@@ -21634,7 +21634,7 @@
         <v>42276.71943287037</v>
       </c>
     </row>
-    <row r="608" spans="1:6">
+    <row r="608" spans="1:6" ht="30">
       <c r="A608" s="1" t="s">
         <v>92</v>
       </c>
@@ -21674,7 +21674,7 @@
         <v>42276.908738425926</v>
       </c>
     </row>
-    <row r="610" spans="1:6">
+    <row r="610" spans="1:6" ht="30">
       <c r="A610" s="1" t="s">
         <v>88</v>
       </c>
@@ -21694,7 +21694,7 @@
         <v>42276.910879629628</v>
       </c>
     </row>
-    <row r="611" spans="1:6">
+    <row r="611" spans="1:6" ht="30">
       <c r="A611" s="1" t="s">
         <v>85</v>
       </c>
@@ -21814,7 +21814,7 @@
         <v>42277.441354166665</v>
       </c>
     </row>
-    <row r="617" spans="1:6">
+    <row r="617" spans="1:6" ht="30">
       <c r="A617" s="1" t="s">
         <v>65</v>
       </c>
@@ -21994,7 +21994,7 @@
         <v>42277.590254629627</v>
       </c>
     </row>
-    <row r="626" spans="1:6">
+    <row r="626" spans="1:6" ht="30">
       <c r="A626" s="1" t="s">
         <v>37</v>
       </c>
@@ -22034,7 +22034,7 @@
         <v>42277.70584490741</v>
       </c>
     </row>
-    <row r="628" spans="1:6">
+    <row r="628" spans="1:6" ht="30">
       <c r="A628" s="1" t="s">
         <v>29</v>
       </c>
@@ -22054,7 +22054,7 @@
         <v>42277.719467592593</v>
       </c>
     </row>
-    <row r="629" spans="1:6">
+    <row r="629" spans="1:6" ht="30">
       <c r="A629" s="1" t="s">
         <v>26</v>
       </c>
@@ -22094,7 +22094,7 @@
         <v>42277.867222222223</v>
       </c>
     </row>
-    <row r="631" spans="1:6">
+    <row r="631" spans="1:6" ht="30">
       <c r="A631" s="1" t="s">
         <v>17</v>
       </c>
@@ -22176,7 +22176,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>